<commit_message>
엑셀 cell merge 같은 값
</commit_message>
<xml_diff>
--- a/WPF_Tranning/HelloWorld.xlsx
+++ b/WPF_Tranning/HelloWorld.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <x:si>
     <x:t>Hello World!</x:t>
   </x:si>
   <x:si>
     <x:t>와우</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -370,7 +373,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:C4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -389,9 +392,15 @@
         <x:f>MID(A1, 7, 6)</x:f>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
-  <x:mergeCells count="1">
+  <x:mergeCells count="2">
     <x:mergeCell ref="C1:D2"/>
+    <x:mergeCell ref="A3:A4"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
list 줄바꾸기, 엑셀 export
</commit_message>
<xml_diff>
--- a/WPF_Tranning/HelloWorld.xlsx
+++ b/WPF_Tranning/HelloWorld.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <x:si>
     <x:t>Hello World!</x:t>
   </x:si>
@@ -37,10 +37,26 @@
     <x:t>def</x:t>
   </x:si>
   <x:si>
+    <x:t>테스트 
+데이터 벨류 : 1234</x:t>
+  </x:si>
+  <x:si>
     <x:t>설치1과</x:t>
   </x:si>
   <x:si>
+    <x:t>데이터 
+벨류2 : 5678</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 
+벨류3 : 9,10,11,12</x:t>
+  </x:si>
+  <x:si>
     <x:t>공백</x:t>
+  </x:si>
+  <x:si>
+    <x:t>데이터 
+벨류4 : 13,14,15,16</x:t>
   </x:si>
   <x:si>
     <x:t>머지방해 데이터</x:t>
@@ -177,7 +193,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="6">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -188,6 +204,10 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -539,98 +559,110 @@
       <x:c r="B11" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="E11" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
-      <x:c r="A12" s="3" t="s">
-        <x:v>7</x:v>
+      <x:c r="A12" s="4" t="s">
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="E12" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
-      <x:c r="A13" s="3" t="s"/>
+      <x:c r="A13" s="4" t="s"/>
       <x:c r="B13" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="E13" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
-      <x:c r="A14" s="3" t="s"/>
-      <x:c r="B14" s="4" t="s">
-        <x:v>8</x:v>
+      <x:c r="A14" s="4" t="s"/>
+      <x:c r="B14" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E14" s="3" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="A15" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
-      <x:c r="A16" s="3" t="s">
+      <x:c r="A16" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:5">
+      <x:c r="A17" s="4" t="s"/>
+      <x:c r="B17" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5">
+      <x:c r="A18" s="4" t="s"/>
+      <x:c r="B18" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="A19" s="4" t="s"/>
+      <x:c r="B19" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5">
+      <x:c r="A20" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B20" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="A21" s="4" t="s"/>
+      <x:c r="B21" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:5">
+      <x:c r="A22" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B22" s="6" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B16" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5">
-      <x:c r="A17" s="3" t="s"/>
-      <x:c r="B17" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="A18" s="3" t="s"/>
-      <x:c r="B18" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5">
-      <x:c r="A19" s="3" t="s"/>
-      <x:c r="B19" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5">
-      <x:c r="A20" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B20" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="A21" s="3" t="s"/>
-      <x:c r="B21" s="1" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:5">
-      <x:c r="A22" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B22" s="5" t="s">
-        <x:v>8</x:v>
-      </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
-      <x:c r="A23" s="3" t="s"/>
+      <x:c r="A23" s="4" t="s"/>
       <x:c r="B23" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
-      <x:c r="A24" s="3" t="s"/>
+      <x:c r="A24" s="4" t="s"/>
       <x:c r="B24" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
-      <x:c r="B25" s="4" t="s">
-        <x:v>8</x:v>
+      <x:c r="B25" s="5" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>